<commit_message>
Update README_raw to include intermediate files
</commit_message>
<xml_diff>
--- a/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
+++ b/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC9267C1-1538-469E-87DF-041C09300799}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output-wrangling-2x2_monitor-in" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={AB11996E-3913-4E9E-BF2E-4C79DED47262}</author>
+    <author>tc={F657FC46-A72A-4BDF-8F6B-4014536F23D7}</author>
     <author>tc={06CE977F-9A9B-4AA1-8ABD-E5C6DF7459F4}</author>
     <author>tc={27F3B0AA-036F-4CCE-AD66-4C3B7713CACF}</author>
     <author>tc={3A16BA3C-8F6C-4C03-83C8-BE9D232F6C33}</author>
@@ -32,7 +33,7 @@
     <author>tc={20D10316-DDDD-4B4D-BC95-1D24F680103B}</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -40,7 +41,15 @@
     Everywhere else says 6/12</t>
       </text>
     </comment>
-    <comment ref="E3" authorId="1" shapeId="0">
+    <comment ref="F2" authorId="1" shapeId="0" xr:uid="{F657FC46-A72A-4BDF-8F6B-4014536F23D7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Is definitely Cool, because on this monitoring date there are only 3 Cool plots and 5 Warm plots, if this were to stay Warm</t>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -48,7 +57,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B19" authorId="2" shapeId="0">
+    <comment ref="B19" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +65,7 @@
     All other instances for Preserve have Date_Seeded marked as 11/25</t>
       </text>
     </comment>
-    <comment ref="E55" authorId="3" shapeId="0">
+    <comment ref="E55" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +73,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B64" authorId="4" shapeId="0">
+    <comment ref="B64" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -72,7 +81,7 @@
     All other instances of Date_Seeded for Roosevelt is 11/22</t>
       </text>
     </comment>
-    <comment ref="E100" authorId="5" shapeId="0">
+    <comment ref="E100" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -80,7 +89,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B112" authorId="6" shapeId="0">
+    <comment ref="B112" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -88,7 +97,7 @@
     All other instances of Date_Seeded are 11/21 for SCC</t>
       </text>
     </comment>
-    <comment ref="E148" authorId="7" shapeId="0">
+    <comment ref="E148" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -101,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="19">
   <si>
     <t>Site</t>
   </si>
@@ -125,9 +134,6 @@
   </si>
   <si>
     <t>Pits</t>
-  </si>
-  <si>
-    <t>Med-Warm</t>
   </si>
   <si>
     <t>Pleasant</t>
@@ -166,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1118,6 +1124,9 @@
   <threadedComment ref="C2" dT="2022-12-09T23:23:04.39" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{AB11996E-3913-4E9E-BF2E-4C79DED47262}">
     <text>Everywhere else says 6/12</text>
   </threadedComment>
+  <threadedComment ref="F2" dT="2022-12-09T03:01:27.83" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{F657FC46-A72A-4BDF-8F6B-4014536F23D7}">
+    <text>Is definitely Cool, because on this monitoring date there are only 3 Cool plots and 5 Warm plots, if this were to stay Warm</text>
+  </threadedComment>
   <threadedComment ref="E3" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{06CE977F-9A9B-4AA1-8ABD-E5C6DF7459F4}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
@@ -1143,12 +1152,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,13 +1202,13 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>43818</v>
@@ -1211,15 +1220,15 @@
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>43818</v>
@@ -1231,15 +1240,15 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>43818</v>
@@ -1251,15 +1260,15 @@
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>43818</v>
@@ -1271,15 +1280,15 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>43818</v>
@@ -1291,15 +1300,15 @@
         <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>43818</v>
@@ -1311,15 +1320,15 @@
         <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>43818</v>
@@ -1331,15 +1340,15 @@
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>43818</v>
@@ -1351,15 +1360,15 @@
         <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>43818</v>
@@ -1371,15 +1380,15 @@
         <v>4</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>43818</v>
@@ -1391,15 +1400,15 @@
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1">
         <v>43818</v>
@@ -1411,15 +1420,15 @@
         <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1">
         <v>43818</v>
@@ -1431,15 +1440,15 @@
         <v>15</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1">
         <v>43818</v>
@@ -1451,15 +1460,15 @@
         <v>22</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1">
         <v>43818</v>
@@ -1471,15 +1480,15 @@
         <v>23</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1">
         <v>43818</v>
@@ -1491,15 +1500,15 @@
         <v>30</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1">
         <v>43818</v>
@@ -1511,15 +1520,15 @@
         <v>32</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="2">
         <v>43794</v>
@@ -1531,15 +1540,15 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2">
         <v>43794</v>
@@ -1551,15 +1560,15 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2">
         <v>43794</v>
@@ -1574,12 +1583,12 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="2">
         <v>43794</v>
@@ -1591,15 +1600,15 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2">
         <v>43794</v>
@@ -1611,15 +1620,15 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
         <v>16</v>
-      </c>
-      <c r="F23" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2">
         <v>43794</v>
@@ -1631,15 +1640,15 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="2">
         <v>43794</v>
@@ -1654,12 +1663,12 @@
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="2">
         <v>43794</v>
@@ -1671,15 +1680,15 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
         <v>16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="2">
         <v>43794</v>
@@ -1691,15 +1700,15 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2">
         <v>43794</v>
@@ -1711,15 +1720,15 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2">
         <v>43794</v>
@@ -1731,15 +1740,15 @@
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="2">
         <v>43794</v>
@@ -1751,15 +1760,15 @@
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="2">
         <v>43794</v>
@@ -1771,15 +1780,15 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="2">
         <v>43794</v>
@@ -1791,15 +1800,15 @@
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="2">
         <v>43794</v>
@@ -1811,15 +1820,15 @@
         <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="2">
         <v>43794</v>
@@ -1834,12 +1843,12 @@
         <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2">
         <v>43794</v>
@@ -1851,15 +1860,15 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="2">
         <v>43794</v>
@@ -1874,12 +1883,12 @@
         <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="2">
         <v>43794</v>
@@ -1891,15 +1900,15 @@
         <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" s="2">
         <v>43794</v>
@@ -1911,15 +1920,15 @@
         <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="2">
         <v>43794</v>
@@ -1931,15 +1940,15 @@
         <v>21</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="2">
         <v>43794</v>
@@ -1954,12 +1963,12 @@
         <v>7</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" s="2">
         <v>43794</v>
@@ -1971,15 +1980,15 @@
         <v>23</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2">
         <v>43794</v>
@@ -1991,15 +2000,15 @@
         <v>24</v>
       </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="2">
         <v>43794</v>
@@ -2011,15 +2020,15 @@
         <v>25</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" s="2">
         <v>43794</v>
@@ -2031,15 +2040,15 @@
         <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" s="2">
         <v>43794</v>
@@ -2054,12 +2063,12 @@
         <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" s="2">
         <v>43794</v>
@@ -2071,15 +2080,15 @@
         <v>28</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47" s="2">
         <v>43794</v>
@@ -2091,15 +2100,15 @@
         <v>29</v>
       </c>
       <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
         <v>16</v>
-      </c>
-      <c r="F47" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B48" s="2">
         <v>43794</v>
@@ -2114,12 +2123,12 @@
         <v>7</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49" s="2">
         <v>43794</v>
@@ -2131,15 +2140,15 @@
         <v>31</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50" s="2">
         <v>43794</v>
@@ -2151,15 +2160,15 @@
         <v>32</v>
       </c>
       <c r="E50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51" s="2">
         <v>43794</v>
@@ -2171,15 +2180,15 @@
         <v>33</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B52" s="2">
         <v>43794</v>
@@ -2191,15 +2200,15 @@
         <v>34</v>
       </c>
       <c r="E52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B53" s="2">
         <v>43794</v>
@@ -2211,15 +2220,15 @@
         <v>35</v>
       </c>
       <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
         <v>16</v>
-      </c>
-      <c r="F53" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="2">
         <v>43794</v>
@@ -2234,12 +2243,12 @@
         <v>7</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" s="1">
         <v>43794</v>
@@ -2251,15 +2260,15 @@
         <v>2</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B56" s="1">
         <v>43794</v>
@@ -2271,15 +2280,15 @@
         <v>6</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" s="1">
         <v>43794</v>
@@ -2291,15 +2300,15 @@
         <v>10</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58" s="1">
         <v>43794</v>
@@ -2311,15 +2320,15 @@
         <v>11</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59" s="1">
         <v>43794</v>
@@ -2331,15 +2340,15 @@
         <v>15</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B60" s="1">
         <v>43794</v>
@@ -2351,15 +2360,15 @@
         <v>21</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B61" s="1">
         <v>43794</v>
@@ -2371,15 +2380,15 @@
         <v>23</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B62" s="1">
         <v>43794</v>
@@ -2391,15 +2400,15 @@
         <v>32</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" s="1">
         <v>43794</v>
@@ -2411,15 +2420,15 @@
         <v>11</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" s="2">
         <v>43791</v>
@@ -2434,12 +2443,12 @@
         <v>7</v>
       </c>
       <c r="F64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65" s="2">
         <v>43791</v>
@@ -2451,15 +2460,15 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66" s="2">
         <v>43791</v>
@@ -2471,15 +2480,15 @@
         <v>3</v>
       </c>
       <c r="E66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B67" s="2">
         <v>43791</v>
@@ -2491,15 +2500,15 @@
         <v>4</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B68" s="2">
         <v>43791</v>
@@ -2514,12 +2523,12 @@
         <v>7</v>
       </c>
       <c r="F68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B69" s="2">
         <v>43791</v>
@@ -2531,15 +2540,15 @@
         <v>6</v>
       </c>
       <c r="E69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B70" s="2">
         <v>43791</v>
@@ -2551,15 +2560,15 @@
         <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B71" s="2">
         <v>43791</v>
@@ -2574,12 +2583,12 @@
         <v>7</v>
       </c>
       <c r="F71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B72" s="2">
         <v>43791</v>
@@ -2591,15 +2600,15 @@
         <v>9</v>
       </c>
       <c r="E72" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s">
         <v>16</v>
-      </c>
-      <c r="F72" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B73" s="2">
         <v>43791</v>
@@ -2611,15 +2620,15 @@
         <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B74" s="2">
         <v>43791</v>
@@ -2631,15 +2640,15 @@
         <v>11</v>
       </c>
       <c r="E74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B75" s="2">
         <v>43791</v>
@@ -2651,15 +2660,15 @@
         <v>12</v>
       </c>
       <c r="E75" t="s">
+        <v>15</v>
+      </c>
+      <c r="F75" t="s">
         <v>16</v>
-      </c>
-      <c r="F75" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B76" s="2">
         <v>43791</v>
@@ -2674,12 +2683,12 @@
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B77" s="2">
         <v>43791</v>
@@ -2691,15 +2700,15 @@
         <v>14</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B78" s="2">
         <v>43791</v>
@@ -2711,15 +2720,15 @@
         <v>15</v>
       </c>
       <c r="E78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B79" s="2">
         <v>43791</v>
@@ -2731,15 +2740,15 @@
         <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B80" s="2">
         <v>43791</v>
@@ -2754,12 +2763,12 @@
         <v>7</v>
       </c>
       <c r="F80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B81" s="2">
         <v>43791</v>
@@ -2771,15 +2780,15 @@
         <v>18</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B82" s="2">
         <v>43791</v>
@@ -2791,15 +2800,15 @@
         <v>19</v>
       </c>
       <c r="E82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B83" s="2">
         <v>43791</v>
@@ -2811,15 +2820,15 @@
         <v>20</v>
       </c>
       <c r="E83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B84" s="2">
         <v>43791</v>
@@ -2834,12 +2843,12 @@
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B85" s="2">
         <v>43791</v>
@@ -2851,15 +2860,15 @@
         <v>22</v>
       </c>
       <c r="E85" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B86" s="2">
         <v>43791</v>
@@ -2871,15 +2880,15 @@
         <v>23</v>
       </c>
       <c r="E86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F86" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B87" s="2">
         <v>43791</v>
@@ -2891,15 +2900,15 @@
         <v>24</v>
       </c>
       <c r="E87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B88" s="2">
         <v>43791</v>
@@ -2911,15 +2920,15 @@
         <v>25</v>
       </c>
       <c r="E88" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" t="s">
         <v>16</v>
-      </c>
-      <c r="F88" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B89" s="2">
         <v>43791</v>
@@ -2931,15 +2940,15 @@
         <v>26</v>
       </c>
       <c r="E89" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B90" s="2">
         <v>43791</v>
@@ -2954,12 +2963,12 @@
         <v>7</v>
       </c>
       <c r="F90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B91" s="2">
         <v>43791</v>
@@ -2971,15 +2980,15 @@
         <v>28</v>
       </c>
       <c r="E91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B92" s="2">
         <v>43791</v>
@@ -2991,15 +3000,15 @@
         <v>29</v>
       </c>
       <c r="E92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B93" s="2">
         <v>43791</v>
@@ -3011,15 +3020,15 @@
         <v>30</v>
       </c>
       <c r="E93" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B94" s="2">
         <v>43791</v>
@@ -3031,15 +3040,15 @@
         <v>31</v>
       </c>
       <c r="E94" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B95" s="2">
         <v>43791</v>
@@ -3051,15 +3060,15 @@
         <v>32</v>
       </c>
       <c r="E95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B96" s="2">
         <v>43791</v>
@@ -3074,12 +3083,12 @@
         <v>7</v>
       </c>
       <c r="F96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B97" s="2">
         <v>43791</v>
@@ -3091,15 +3100,15 @@
         <v>34</v>
       </c>
       <c r="E97" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B98" s="2">
         <v>43791</v>
@@ -3111,15 +3120,15 @@
         <v>35</v>
       </c>
       <c r="E98" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" t="s">
         <v>16</v>
-      </c>
-      <c r="F98" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B99" s="2">
         <v>43791</v>
@@ -3131,15 +3140,15 @@
         <v>36</v>
       </c>
       <c r="E99" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B100" s="1">
         <v>43791</v>
@@ -3151,15 +3160,15 @@
         <v>2</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B101" s="1">
         <v>43791</v>
@@ -3171,15 +3180,15 @@
         <v>7</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B102" s="1">
         <v>43791</v>
@@ -3191,15 +3200,15 @@
         <v>11</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B103" s="1">
         <v>43791</v>
@@ -3211,15 +3220,15 @@
         <v>16</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B104" s="1">
         <v>43791</v>
@@ -3231,15 +3240,15 @@
         <v>20</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F104" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B105" s="1">
         <v>43791</v>
@@ -3251,15 +3260,15 @@
         <v>30</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B106" s="1">
         <v>43791</v>
@@ -3271,15 +3280,15 @@
         <v>34</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B107" s="1">
         <v>43791</v>
@@ -3291,15 +3300,15 @@
         <v>36</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B108" s="1">
         <v>43791</v>
@@ -3311,15 +3320,15 @@
         <v>2</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B109" s="1">
         <v>43791</v>
@@ -3331,15 +3340,15 @@
         <v>16</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B110" s="1">
         <v>43791</v>
@@ -3351,15 +3360,15 @@
         <v>30</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F110" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B111" s="1">
         <v>43791</v>
@@ -3371,15 +3380,15 @@
         <v>34</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B112" s="2">
         <v>43790</v>
@@ -3391,15 +3400,15 @@
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B113" s="2">
         <v>43790</v>
@@ -3411,15 +3420,15 @@
         <v>2</v>
       </c>
       <c r="E113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B114" s="2">
         <v>43790</v>
@@ -3431,15 +3440,15 @@
         <v>3</v>
       </c>
       <c r="E114" t="s">
+        <v>15</v>
+      </c>
+      <c r="F114" t="s">
         <v>16</v>
-      </c>
-      <c r="F114" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B115" s="2">
         <v>43790</v>
@@ -3451,15 +3460,15 @@
         <v>4</v>
       </c>
       <c r="E115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B116" s="2">
         <v>43790</v>
@@ -3474,12 +3483,12 @@
         <v>7</v>
       </c>
       <c r="F116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B117" s="2">
         <v>43790</v>
@@ -3491,15 +3500,15 @@
         <v>6</v>
       </c>
       <c r="E117" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F117" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B118" s="2">
         <v>43790</v>
@@ -3511,15 +3520,15 @@
         <v>7</v>
       </c>
       <c r="E118" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F118" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B119" s="2">
         <v>43790</v>
@@ -3531,15 +3540,15 @@
         <v>8</v>
       </c>
       <c r="E119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B120" s="2">
         <v>43790</v>
@@ -3551,15 +3560,15 @@
         <v>9</v>
       </c>
       <c r="E120" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B121" s="2">
         <v>43790</v>
@@ -3574,12 +3583,12 @@
         <v>7</v>
       </c>
       <c r="F121" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B122" s="2">
         <v>43790</v>
@@ -3591,15 +3600,15 @@
         <v>11</v>
       </c>
       <c r="E122" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F122" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B123" s="2">
         <v>43790</v>
@@ -3611,15 +3620,15 @@
         <v>12</v>
       </c>
       <c r="E123" t="s">
+        <v>15</v>
+      </c>
+      <c r="F123" t="s">
         <v>16</v>
-      </c>
-      <c r="F123" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B124" s="2">
         <v>43790</v>
@@ -3631,15 +3640,15 @@
         <v>13</v>
       </c>
       <c r="E124" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F124" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B125" s="2">
         <v>43790</v>
@@ -3651,15 +3660,15 @@
         <v>14</v>
       </c>
       <c r="E125" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B126" s="2">
         <v>43790</v>
@@ -3671,15 +3680,15 @@
         <v>15</v>
       </c>
       <c r="E126" t="s">
+        <v>15</v>
+      </c>
+      <c r="F126" t="s">
         <v>16</v>
-      </c>
-      <c r="F126" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B127" s="2">
         <v>43790</v>
@@ -3691,15 +3700,15 @@
         <v>16</v>
       </c>
       <c r="E127" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F127" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B128" s="2">
         <v>43790</v>
@@ -3711,15 +3720,15 @@
         <v>17</v>
       </c>
       <c r="E128" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B129" s="2">
         <v>43790</v>
@@ -3734,12 +3743,12 @@
         <v>7</v>
       </c>
       <c r="F129" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B130" s="2">
         <v>43790</v>
@@ -3751,15 +3760,15 @@
         <v>19</v>
       </c>
       <c r="E130" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F130" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B131" s="2">
         <v>43790</v>
@@ -3771,15 +3780,15 @@
         <v>20</v>
       </c>
       <c r="E131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F131" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B132" s="2">
         <v>43790</v>
@@ -3794,12 +3803,12 @@
         <v>7</v>
       </c>
       <c r="F132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B133" s="2">
         <v>43790</v>
@@ -3811,15 +3820,15 @@
         <v>22</v>
       </c>
       <c r="E133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F133" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B134" s="2">
         <v>43790</v>
@@ -3831,15 +3840,15 @@
         <v>23</v>
       </c>
       <c r="E134" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B135" s="2">
         <v>43790</v>
@@ -3854,12 +3863,12 @@
         <v>7</v>
       </c>
       <c r="F135" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B136" s="2">
         <v>43790</v>
@@ -3871,15 +3880,15 @@
         <v>25</v>
       </c>
       <c r="E136" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F136" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B137" s="2">
         <v>43790</v>
@@ -3891,15 +3900,15 @@
         <v>26</v>
       </c>
       <c r="E137" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F137" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B138" s="2">
         <v>43790</v>
@@ -3911,15 +3920,15 @@
         <v>27</v>
       </c>
       <c r="E138" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F138" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B139" s="2">
         <v>43790</v>
@@ -3934,12 +3943,12 @@
         <v>7</v>
       </c>
       <c r="F139" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B140" s="2">
         <v>43790</v>
@@ -3951,15 +3960,15 @@
         <v>29</v>
       </c>
       <c r="E140" t="s">
+        <v>15</v>
+      </c>
+      <c r="F140" t="s">
         <v>16</v>
-      </c>
-      <c r="F140" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B141" s="2">
         <v>43790</v>
@@ -3971,15 +3980,15 @@
         <v>30</v>
       </c>
       <c r="E141" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F141" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B142" s="2">
         <v>43790</v>
@@ -3994,12 +4003,12 @@
         <v>7</v>
       </c>
       <c r="F142" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B143" s="2">
         <v>43790</v>
@@ -4011,15 +4020,15 @@
         <v>32</v>
       </c>
       <c r="E143" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F143" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B144" s="2">
         <v>43790</v>
@@ -4031,15 +4040,15 @@
         <v>33</v>
       </c>
       <c r="E144" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B145" s="2">
         <v>43790</v>
@@ -4051,15 +4060,15 @@
         <v>34</v>
       </c>
       <c r="E145" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F145" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B146" s="2">
         <v>43790</v>
@@ -4071,15 +4080,15 @@
         <v>35</v>
       </c>
       <c r="E146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F146" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B147" s="2">
         <v>43790</v>
@@ -4094,12 +4103,12 @@
         <v>7</v>
       </c>
       <c r="F147" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B148" s="2">
         <v>43790</v>
@@ -4111,15 +4120,15 @@
         <v>4</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F148" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B149" s="1">
         <v>43790</v>
@@ -4131,15 +4140,15 @@
         <v>8</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F149" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B150" s="1">
         <v>43790</v>
@@ -4151,15 +4160,15 @@
         <v>13</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F150" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B151" s="1">
         <v>43790</v>
@@ -4171,15 +4180,15 @@
         <v>16</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F151" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B152" s="1">
         <v>43790</v>
@@ -4191,15 +4200,15 @@
         <v>22</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F152" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B153" s="1">
         <v>43790</v>
@@ -4211,15 +4220,15 @@
         <v>25</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F153" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B154" s="1">
         <v>43790</v>
@@ -4231,15 +4240,15 @@
         <v>32</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F154" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B155" s="1">
         <v>43790</v>
@@ -4251,15 +4260,15 @@
         <v>35</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F155" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B156" s="1">
         <v>43790</v>
@@ -4271,15 +4280,15 @@
         <v>16</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F156" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B157" s="1">
         <v>43790</v>
@@ -4291,15 +4300,15 @@
         <v>25</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F157" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B158" s="1">
         <v>43790</v>
@@ -4311,10 +4320,10 @@
         <v>35</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally fixed the issue with FlyingM and changing its Date_Seeded for all observations
</commit_message>
<xml_diff>
--- a/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
+++ b/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC9267C1-1538-469E-87DF-041C09300799}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17878EB4-8906-403A-B63E-9D57F9403AFD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6528" yWindow="3960" windowWidth="17208" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="output-wrangling-2x2_monitor-in" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,8 +22,8 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={C2A3709D-DE0C-4601-A84E-C52536182A79}</author>
     <author>tc={AB11996E-3913-4E9E-BF2E-4C79DED47262}</author>
-    <author>tc={F657FC46-A72A-4BDF-8F6B-4014536F23D7}</author>
     <author>tc={06CE977F-9A9B-4AA1-8ABD-E5C6DF7459F4}</author>
     <author>tc={27F3B0AA-036F-4CCE-AD66-4C3B7713CACF}</author>
     <author>tc={3A16BA3C-8F6C-4C03-83C8-BE9D232F6C33}</author>
@@ -33,20 +33,20 @@
     <author>tc={20D10316-DDDD-4B4D-BC95-1D24F680103B}</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{C2A3709D-DE0C-4601-A84E-C52536182A79}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    FlyingM was seeded on 7/17 and 7/18. Every other observation for the 6/12/19 monitoring date has the Date_Seeded as 7/18.</t>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Everywhere else says 6/12</t>
-      </text>
-    </comment>
-    <comment ref="F2" authorId="1" shapeId="0" xr:uid="{F657FC46-A72A-4BDF-8F6B-4014536F23D7}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Is definitely Cool, because on this monitoring date there are only 3 Cool plots and 5 Warm plots, if this were to stay Warm</t>
       </text>
     </comment>
     <comment ref="E3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="20">
   <si>
     <t>Site</t>
   </si>
@@ -168,12 +168,15 @@
   <si>
     <t>SCC</t>
   </si>
+  <si>
+    <t>Med-Warm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,12 +310,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1121,11 +1118,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2022-12-10T05:26:11.76" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{C2A3709D-DE0C-4601-A84E-C52536182A79}">
+    <text>FlyingM was seeded on 7/17 and 7/18. Every other observation for the 6/12/19 monitoring date has the Date_Seeded as 7/18.</text>
+  </threadedComment>
   <threadedComment ref="C2" dT="2022-12-09T23:23:04.39" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{AB11996E-3913-4E9E-BF2E-4C79DED47262}">
     <text>Everywhere else says 6/12</text>
-  </threadedComment>
-  <threadedComment ref="F2" dT="2022-12-09T03:01:27.83" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{F657FC46-A72A-4BDF-8F6B-4014536F23D7}">
-    <text>Is definitely Cool, because on this monitoring date there are only 3 Cool plots and 5 Warm plots, if this were to stay Warm</text>
   </threadedComment>
   <threadedComment ref="E3" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{06CE977F-9A9B-4AA1-8ABD-E5C6DF7459F4}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
@@ -1157,7 +1154,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,8 +1187,8 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
-        <v>43306</v>
+      <c r="B2" s="2">
+        <v>43299</v>
       </c>
       <c r="C2" s="2">
         <v>43628</v>
@@ -1202,8 +1199,8 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
+      <c r="F2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix location-dependent and location-independent species lists. I think they got messed up because I kept piping the object into an object of the same name, so it overwrote itself many times, versus starting from scratch when something didn't work
</commit_message>
<xml_diff>
--- a/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
+++ b/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17878EB4-8906-403A-B63E-9D57F9403AFD}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FA09BC-BFB1-4E92-901A-0CB3AA5B6DFA}"/>
   <bookViews>
-    <workbookView xWindow="6528" yWindow="3960" windowWidth="17208" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="12408" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B19" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B18" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -65,7 +65,7 @@
     All other instances for Preserve have Date_Seeded marked as 11/25</t>
       </text>
     </comment>
-    <comment ref="E55" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="E54" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -73,7 +73,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B64" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B63" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -81,7 +81,7 @@
     All other instances of Date_Seeded for Roosevelt is 11/22</t>
       </text>
     </comment>
-    <comment ref="E100" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="E99" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -89,7 +89,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B112" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B111" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -97,7 +97,7 @@
     All other instances of Date_Seeded are 11/21 for SCC</t>
       </text>
     </comment>
-    <comment ref="E148" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="E147" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="20">
   <si>
     <t>Site</t>
   </si>
@@ -734,7 +734,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1127,22 +1127,22 @@
   <threadedComment ref="E3" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{06CE977F-9A9B-4AA1-8ABD-E5C6DF7459F4}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
-  <threadedComment ref="B19" dT="2022-12-09T23:24:10.06" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{27F3B0AA-036F-4CCE-AD66-4C3B7713CACF}">
+  <threadedComment ref="B18" dT="2022-12-09T23:24:10.06" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{27F3B0AA-036F-4CCE-AD66-4C3B7713CACF}">
     <text>All other instances for Preserve have Date_Seeded marked as 11/25</text>
   </threadedComment>
-  <threadedComment ref="E55" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{3A16BA3C-8F6C-4C03-83C8-BE9D232F6C33}">
+  <threadedComment ref="E54" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{3A16BA3C-8F6C-4C03-83C8-BE9D232F6C33}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
-  <threadedComment ref="B64" dT="2022-12-09T23:24:59.41" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{28A7DFF1-32AB-4630-99DC-BF5D69F548F5}">
+  <threadedComment ref="B63" dT="2022-12-09T23:24:59.41" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{28A7DFF1-32AB-4630-99DC-BF5D69F548F5}">
     <text>All other instances of Date_Seeded for Roosevelt is 11/22</text>
   </threadedComment>
-  <threadedComment ref="E100" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{943D5A63-B839-4548-972B-FF09A35598FA}">
+  <threadedComment ref="E99" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{943D5A63-B839-4548-972B-FF09A35598FA}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
-  <threadedComment ref="B112" dT="2022-12-09T23:25:43.36" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{48C8DF8B-6279-4847-B5FA-E3FCAC2F369F}">
+  <threadedComment ref="B111" dT="2022-12-09T23:25:43.36" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{48C8DF8B-6279-4847-B5FA-E3FCAC2F369F}">
     <text>All other instances of Date_Seeded are 11/21 for SCC</text>
   </threadedComment>
-  <threadedComment ref="E148" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{20D10316-DDDD-4B4D-BC95-1D24F680103B}">
+  <threadedComment ref="E147" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{20D10316-DDDD-4B4D-BC95-1D24F680103B}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
 </ThreadedComments>
@@ -1150,11 +1150,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1294,13 +1294,13 @@
         <v>44288</v>
       </c>
       <c r="D7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1314,13 +1314,13 @@
         <v>44288</v>
       </c>
       <c r="D8">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1334,13 +1334,13 @@
         <v>44288</v>
       </c>
       <c r="D9">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1351,16 +1351,16 @@
         <v>43818</v>
       </c>
       <c r="C10" s="1">
-        <v>44288</v>
+        <v>44473</v>
       </c>
       <c r="D10">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1374,13 +1374,13 @@
         <v>44473</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1394,13 +1394,13 @@
         <v>44473</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1414,13 +1414,13 @@
         <v>44473</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1434,13 +1434,13 @@
         <v>44473</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1454,13 +1454,13 @@
         <v>44473</v>
       </c>
       <c r="D15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1474,13 +1474,13 @@
         <v>44473</v>
       </c>
       <c r="D16">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1494,30 +1494,30 @@
         <v>44473</v>
       </c>
       <c r="D17">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1">
-        <v>43818</v>
+        <v>11</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43794</v>
       </c>
       <c r="C18" s="1">
-        <v>44473</v>
+        <v>43916</v>
       </c>
       <c r="D18">
-        <v>32</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
@@ -1534,10 +1534,10 @@
         <v>43916</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -1554,10 +1554,10 @@
         <v>43916</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
@@ -1574,10 +1574,10 @@
         <v>43916</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
@@ -1594,13 +1594,13 @@
         <v>43916</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1614,13 +1614,13 @@
         <v>43916</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1634,10 +1634,10 @@
         <v>43916</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
@@ -1654,13 +1654,13 @@
         <v>43916</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1674,13 +1674,13 @@
         <v>43916</v>
       </c>
       <c r="D26">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1694,13 +1694,13 @@
         <v>43916</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1714,13 +1714,13 @@
         <v>43916</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1734,10 +1734,10 @@
         <v>43916</v>
       </c>
       <c r="D29">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
         <v>9</v>
@@ -1754,13 +1754,13 @@
         <v>43916</v>
       </c>
       <c r="D30">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
         <v>12</v>
       </c>
-      <c r="E30" t="s">
-        <v>14</v>
-      </c>
       <c r="F30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1774,10 +1774,10 @@
         <v>43916</v>
       </c>
       <c r="D31">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -1794,10 +1794,10 @@
         <v>43916</v>
       </c>
       <c r="D32">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -1814,10 +1814,10 @@
         <v>43916</v>
       </c>
       <c r="D33">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -1834,13 +1834,13 @@
         <v>43916</v>
       </c>
       <c r="D34">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1854,10 +1854,10 @@
         <v>43916</v>
       </c>
       <c r="D35">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
         <v>9</v>
@@ -1874,10 +1874,10 @@
         <v>43916</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F36" t="s">
         <v>9</v>
@@ -1894,13 +1894,13 @@
         <v>43916</v>
       </c>
       <c r="D37">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1914,13 +1914,13 @@
         <v>43916</v>
       </c>
       <c r="D38">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1934,13 +1934,13 @@
         <v>43916</v>
       </c>
       <c r="D39">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1954,10 +1954,10 @@
         <v>43916</v>
       </c>
       <c r="D40">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
@@ -1974,13 +1974,13 @@
         <v>43916</v>
       </c>
       <c r="D41">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1994,13 +1994,13 @@
         <v>43916</v>
       </c>
       <c r="D42">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2014,10 +2014,10 @@
         <v>43916</v>
       </c>
       <c r="D43">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F43" t="s">
         <v>10</v>
@@ -2034,13 +2034,13 @@
         <v>43916</v>
       </c>
       <c r="D44">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E44" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2054,10 +2054,10 @@
         <v>43916</v>
       </c>
       <c r="D45">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F45" t="s">
         <v>9</v>
@@ -2074,13 +2074,13 @@
         <v>43916</v>
       </c>
       <c r="D46">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2094,13 +2094,13 @@
         <v>43916</v>
       </c>
       <c r="D47">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2114,10 +2114,10 @@
         <v>43916</v>
       </c>
       <c r="D48">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
         <v>10</v>
@@ -2134,13 +2134,13 @@
         <v>43916</v>
       </c>
       <c r="D49">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2154,10 +2154,10 @@
         <v>43916</v>
       </c>
       <c r="D50">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
         <v>9</v>
@@ -2174,10 +2174,10 @@
         <v>43916</v>
       </c>
       <c r="D51">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
         <v>9</v>
@@ -2194,13 +2194,13 @@
         <v>43916</v>
       </c>
       <c r="D52">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2214,33 +2214,33 @@
         <v>43916</v>
       </c>
       <c r="D53">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E53" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>11</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>43794</v>
       </c>
       <c r="C54" s="1">
-        <v>43916</v>
+        <v>44285</v>
       </c>
       <c r="D54">
-        <v>36</v>
-      </c>
-      <c r="E54" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="F54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2254,13 +2254,13 @@
         <v>44285</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2274,13 +2274,13 @@
         <v>44285</v>
       </c>
       <c r="D56">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2294,13 +2294,13 @@
         <v>44285</v>
       </c>
       <c r="D57">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2314,13 +2314,13 @@
         <v>44285</v>
       </c>
       <c r="D58">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2334,13 +2334,13 @@
         <v>44285</v>
       </c>
       <c r="D59">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2354,13 +2354,13 @@
         <v>44285</v>
       </c>
       <c r="D60">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2374,13 +2374,13 @@
         <v>44285</v>
       </c>
       <c r="D61">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2391,10 +2391,10 @@
         <v>43794</v>
       </c>
       <c r="C62" s="1">
-        <v>44285</v>
+        <v>44475</v>
       </c>
       <c r="D62">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>13</v>
@@ -2405,22 +2405,22 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B63" s="1">
-        <v>43794</v>
+        <v>17</v>
+      </c>
+      <c r="B63" s="2">
+        <v>43791</v>
       </c>
       <c r="C63" s="1">
-        <v>44475</v>
+        <v>43915</v>
       </c>
       <c r="D63">
-        <v>11</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>7</v>
       </c>
       <c r="F63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2434,10 +2434,10 @@
         <v>43915</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F64" t="s">
         <v>10</v>
@@ -2454,10 +2454,10 @@
         <v>43915</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F65" t="s">
         <v>10</v>
@@ -2474,10 +2474,10 @@
         <v>43915</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F66" t="s">
         <v>10</v>
@@ -2494,13 +2494,13 @@
         <v>43915</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E67" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2514,10 +2514,10 @@
         <v>43915</v>
       </c>
       <c r="D68">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E68" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F68" t="s">
         <v>9</v>
@@ -2534,10 +2534,10 @@
         <v>43915</v>
       </c>
       <c r="D69">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F69" t="s">
         <v>9</v>
@@ -2554,13 +2554,13 @@
         <v>43915</v>
       </c>
       <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
         <v>7</v>
       </c>
-      <c r="E70" t="s">
-        <v>13</v>
-      </c>
       <c r="F70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2574,13 +2574,13 @@
         <v>43915</v>
       </c>
       <c r="D71">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E71" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F71" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2594,13 +2594,13 @@
         <v>43915</v>
       </c>
       <c r="D72">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F72" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2614,13 +2614,13 @@
         <v>43915</v>
       </c>
       <c r="D73">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2634,13 +2634,13 @@
         <v>43915</v>
       </c>
       <c r="D74">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2654,13 +2654,13 @@
         <v>43915</v>
       </c>
       <c r="D75">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E75" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F75" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2674,10 +2674,10 @@
         <v>43915</v>
       </c>
       <c r="D76">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E76" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F76" t="s">
         <v>9</v>
@@ -2694,13 +2694,13 @@
         <v>43915</v>
       </c>
       <c r="D77">
+        <v>15</v>
+      </c>
+      <c r="E77" t="s">
         <v>14</v>
       </c>
-      <c r="E77" t="s">
-        <v>12</v>
-      </c>
       <c r="F77" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2714,13 +2714,13 @@
         <v>43915</v>
       </c>
       <c r="D78">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2734,13 +2734,13 @@
         <v>43915</v>
       </c>
       <c r="D79">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F79" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2754,10 +2754,10 @@
         <v>43915</v>
       </c>
       <c r="D80">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E80" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F80" t="s">
         <v>10</v>
@@ -2774,10 +2774,10 @@
         <v>43915</v>
       </c>
       <c r="D81">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F81" t="s">
         <v>10</v>
@@ -2794,10 +2794,10 @@
         <v>43915</v>
       </c>
       <c r="D82">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F82" t="s">
         <v>10</v>
@@ -2814,13 +2814,13 @@
         <v>43915</v>
       </c>
       <c r="D83">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E83" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2834,10 +2834,10 @@
         <v>43915</v>
       </c>
       <c r="D84">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E84" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F84" t="s">
         <v>9</v>
@@ -2854,13 +2854,13 @@
         <v>43915</v>
       </c>
       <c r="D85">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E85" t="s">
         <v>12</v>
       </c>
       <c r="F85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2874,13 +2874,13 @@
         <v>43915</v>
       </c>
       <c r="D86">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E86" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2894,13 +2894,13 @@
         <v>43915</v>
       </c>
       <c r="D87">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E87" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F87" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2914,13 +2914,13 @@
         <v>43915</v>
       </c>
       <c r="D88">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E88" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F88" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2934,13 +2934,13 @@
         <v>43915</v>
       </c>
       <c r="D89">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E89" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -2954,10 +2954,10 @@
         <v>43915</v>
       </c>
       <c r="D90">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E90" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F90" t="s">
         <v>10</v>
@@ -2974,10 +2974,10 @@
         <v>43915</v>
       </c>
       <c r="D91">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E91" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F91" t="s">
         <v>10</v>
@@ -2994,13 +2994,13 @@
         <v>43915</v>
       </c>
       <c r="D92">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E92" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -3014,10 +3014,10 @@
         <v>43915</v>
       </c>
       <c r="D93">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F93" t="s">
         <v>9</v>
@@ -3034,10 +3034,10 @@
         <v>43915</v>
       </c>
       <c r="D94">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E94" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F94" t="s">
         <v>9</v>
@@ -3054,10 +3054,10 @@
         <v>43915</v>
       </c>
       <c r="D95">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E95" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F95" t="s">
         <v>9</v>
@@ -3074,13 +3074,13 @@
         <v>43915</v>
       </c>
       <c r="D96">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E96" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -3094,13 +3094,13 @@
         <v>43915</v>
       </c>
       <c r="D97">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E97" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F97" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -3114,33 +3114,33 @@
         <v>43915</v>
       </c>
       <c r="D98">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E98" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F98" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>17</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="1">
         <v>43791</v>
       </c>
       <c r="C99" s="1">
-        <v>43915</v>
+        <v>44287</v>
       </c>
       <c r="D99">
-        <v>36</v>
-      </c>
-      <c r="E99" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F99" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3154,13 +3154,13 @@
         <v>44287</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3174,13 +3174,13 @@
         <v>44287</v>
       </c>
       <c r="D101">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F101" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3194,13 +3194,13 @@
         <v>44287</v>
       </c>
       <c r="D102">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3214,13 +3214,13 @@
         <v>44287</v>
       </c>
       <c r="D103">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F103" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3234,13 +3234,13 @@
         <v>44287</v>
       </c>
       <c r="D104">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,13 +3254,13 @@
         <v>44287</v>
       </c>
       <c r="D105">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F105" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,13 +3274,13 @@
         <v>44287</v>
       </c>
       <c r="D106">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F106" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3291,16 +3291,16 @@
         <v>43791</v>
       </c>
       <c r="C107" s="1">
-        <v>44287</v>
+        <v>44477</v>
       </c>
       <c r="D107">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F107" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3314,13 +3314,13 @@
         <v>44477</v>
       </c>
       <c r="D108">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -3334,7 +3334,7 @@
         <v>44477</v>
       </c>
       <c r="D109">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>13</v>
@@ -3354,30 +3354,30 @@
         <v>44477</v>
       </c>
       <c r="D110">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F110" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>17</v>
-      </c>
-      <c r="B111" s="1">
-        <v>43791</v>
+        <v>18</v>
+      </c>
+      <c r="B111" s="2">
+        <v>43790</v>
       </c>
       <c r="C111" s="1">
-        <v>44477</v>
+        <v>43917</v>
       </c>
       <c r="D111">
-        <v>34</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>12</v>
       </c>
       <c r="F111" t="s">
         <v>10</v>
@@ -3394,10 +3394,10 @@
         <v>43917</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E112" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F112" t="s">
         <v>10</v>
@@ -3414,13 +3414,13 @@
         <v>43917</v>
       </c>
       <c r="D113">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E113" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F113" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3434,13 +3434,13 @@
         <v>43917</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E114" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F114" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3454,10 +3454,10 @@
         <v>43917</v>
       </c>
       <c r="D115">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E115" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F115" t="s">
         <v>10</v>
@@ -3474,13 +3474,13 @@
         <v>43917</v>
       </c>
       <c r="D116">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E116" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3494,10 +3494,10 @@
         <v>43917</v>
       </c>
       <c r="D117">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E117" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F117" t="s">
         <v>9</v>
@@ -3514,10 +3514,10 @@
         <v>43917</v>
       </c>
       <c r="D118">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E118" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F118" t="s">
         <v>9</v>
@@ -3534,13 +3534,13 @@
         <v>43917</v>
       </c>
       <c r="D119">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E119" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F119" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3554,13 +3554,13 @@
         <v>43917</v>
       </c>
       <c r="D120">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E120" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3574,13 +3574,13 @@
         <v>43917</v>
       </c>
       <c r="D121">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E121" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F121" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3594,13 +3594,13 @@
         <v>43917</v>
       </c>
       <c r="D122">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E122" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F122" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3614,13 +3614,13 @@
         <v>43917</v>
       </c>
       <c r="D123">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E123" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F123" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3634,13 +3634,13 @@
         <v>43917</v>
       </c>
       <c r="D124">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3654,13 +3654,13 @@
         <v>43917</v>
       </c>
       <c r="D125">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E125" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F125" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3674,13 +3674,13 @@
         <v>43917</v>
       </c>
       <c r="D126">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E126" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F126" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3694,10 +3694,10 @@
         <v>43917</v>
       </c>
       <c r="D127">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E127" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F127" t="s">
         <v>9</v>
@@ -3714,13 +3714,13 @@
         <v>43917</v>
       </c>
       <c r="D128">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E128" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F128" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3734,10 +3734,10 @@
         <v>43917</v>
       </c>
       <c r="D129">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E129" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F129" t="s">
         <v>10</v>
@@ -3754,10 +3754,10 @@
         <v>43917</v>
       </c>
       <c r="D130">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E130" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F130" t="s">
         <v>10</v>
@@ -3774,13 +3774,13 @@
         <v>43917</v>
       </c>
       <c r="D131">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E131" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F131" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3794,13 +3794,13 @@
         <v>43917</v>
       </c>
       <c r="D132">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E132" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F132" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3814,13 +3814,13 @@
         <v>43917</v>
       </c>
       <c r="D133">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F133" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3834,13 +3834,13 @@
         <v>43917</v>
       </c>
       <c r="D134">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E134" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F134" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3854,13 +3854,13 @@
         <v>43917</v>
       </c>
       <c r="D135">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E135" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F135" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3874,13 +3874,13 @@
         <v>43917</v>
       </c>
       <c r="D136">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F136" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3894,13 +3894,13 @@
         <v>43917</v>
       </c>
       <c r="D137">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E137" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F137" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3914,10 +3914,10 @@
         <v>43917</v>
       </c>
       <c r="D138">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E138" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F138" t="s">
         <v>9</v>
@@ -3934,13 +3934,13 @@
         <v>43917</v>
       </c>
       <c r="D139">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E139" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F139" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3954,13 +3954,13 @@
         <v>43917</v>
       </c>
       <c r="D140">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E140" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F140" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -3974,10 +3974,10 @@
         <v>43917</v>
       </c>
       <c r="D141">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E141" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F141" t="s">
         <v>10</v>
@@ -3994,10 +3994,10 @@
         <v>43917</v>
       </c>
       <c r="D142">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E142" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F142" t="s">
         <v>10</v>
@@ -4014,13 +4014,13 @@
         <v>43917</v>
       </c>
       <c r="D143">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F143" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -4034,10 +4034,10 @@
         <v>43917</v>
       </c>
       <c r="D144">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E144" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F144" t="s">
         <v>9</v>
@@ -4054,10 +4054,10 @@
         <v>43917</v>
       </c>
       <c r="D145">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E145" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F145" t="s">
         <v>9</v>
@@ -4074,10 +4074,10 @@
         <v>43917</v>
       </c>
       <c r="D146">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E146" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F146" t="s">
         <v>9</v>
@@ -4091,36 +4091,36 @@
         <v>43790</v>
       </c>
       <c r="C147" s="1">
-        <v>43917</v>
+        <v>44286</v>
       </c>
       <c r="D147">
-        <v>36</v>
-      </c>
-      <c r="E147" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="F147" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>18</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148" s="1">
         <v>43790</v>
       </c>
       <c r="C148" s="1">
         <v>44286</v>
       </c>
       <c r="D148">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F148" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -4134,13 +4134,13 @@
         <v>44286</v>
       </c>
       <c r="D149">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F149" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -4154,13 +4154,13 @@
         <v>44286</v>
       </c>
       <c r="D150">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F150" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -4174,13 +4174,13 @@
         <v>44286</v>
       </c>
       <c r="D151">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F151" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -4194,13 +4194,13 @@
         <v>44286</v>
       </c>
       <c r="D152">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F152" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -4214,13 +4214,13 @@
         <v>44286</v>
       </c>
       <c r="D153">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F153" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -4234,13 +4234,13 @@
         <v>44286</v>
       </c>
       <c r="D154">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F154" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -4251,10 +4251,10 @@
         <v>43790</v>
       </c>
       <c r="C155" s="1">
-        <v>44286</v>
+        <v>44482</v>
       </c>
       <c r="D155">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>13</v>
@@ -4274,7 +4274,7 @@
         <v>44482</v>
       </c>
       <c r="D156">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>13</v>
@@ -4294,32 +4294,12 @@
         <v>44482</v>
       </c>
       <c r="D157">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F157" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>18</v>
-      </c>
-      <c r="B158" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C158" s="1">
-        <v>44482</v>
-      </c>
-      <c r="D158">
-        <v>35</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F158" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Monitoring info corrected for 2x2 data
</commit_message>
<xml_diff>
--- a/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
+++ b/data/raw/edited-wrangling-2x2_1monitor-info-fixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FA09BC-BFB1-4E92-901A-0CB3AA5B6DFA}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:40009_{FA99B615-1013-454C-A026-6909C1DFF758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{877227A1-36FE-4EE3-9008-859925347694}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="12408" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="12408" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <author>tc={28A7DFF1-32AB-4630-99DC-BF5D69F548F5}</author>
     <author>tc={943D5A63-B839-4548-972B-FF09A35598FA}</author>
     <author>tc={48C8DF8B-6279-4847-B5FA-E3FCAC2F369F}</author>
-    <author>tc={20D10316-DDDD-4B4D-BC95-1D24F680103B}</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{C2A3709D-DE0C-4601-A84E-C52536182A79}">
@@ -57,7 +56,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B18" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B17" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -65,7 +64,7 @@
     All other instances for Preserve have Date_Seeded marked as 11/25</t>
       </text>
     </comment>
-    <comment ref="E54" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="E53" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -73,7 +72,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B63" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B62" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -81,7 +80,7 @@
     All other instances of Date_Seeded for Roosevelt is 11/22</t>
       </text>
     </comment>
-    <comment ref="E99" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="E98" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -89,7 +88,7 @@
     "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
       </text>
     </comment>
-    <comment ref="B111" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B109" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -97,20 +96,12 @@
     All other instances of Date_Seeded are 11/21 for SCC</t>
       </text>
     </comment>
-    <comment ref="E147" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    "Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="20">
   <si>
     <t>Site</t>
   </si>
@@ -1127,34 +1118,31 @@
   <threadedComment ref="E3" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{06CE977F-9A9B-4AA1-8ABD-E5C6DF7459F4}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
-  <threadedComment ref="B18" dT="2022-12-09T23:24:10.06" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{27F3B0AA-036F-4CCE-AD66-4C3B7713CACF}">
+  <threadedComment ref="B17" dT="2022-12-09T23:24:10.06" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{27F3B0AA-036F-4CCE-AD66-4C3B7713CACF}">
     <text>All other instances for Preserve have Date_Seeded marked as 11/25</text>
   </threadedComment>
-  <threadedComment ref="E54" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{3A16BA3C-8F6C-4C03-83C8-BE9D232F6C33}">
+  <threadedComment ref="E53" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{3A16BA3C-8F6C-4C03-83C8-BE9D232F6C33}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
-  <threadedComment ref="B63" dT="2022-12-09T23:24:59.41" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{28A7DFF1-32AB-4630-99DC-BF5D69F548F5}">
+  <threadedComment ref="B62" dT="2022-12-09T23:24:59.41" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{28A7DFF1-32AB-4630-99DC-BF5D69F548F5}">
     <text>All other instances of Date_Seeded for Roosevelt is 11/22</text>
   </threadedComment>
-  <threadedComment ref="E99" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{943D5A63-B839-4548-972B-FF09A35598FA}">
+  <threadedComment ref="E98" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{943D5A63-B839-4548-972B-FF09A35598FA}">
     <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
-  <threadedComment ref="B111" dT="2022-12-09T23:25:43.36" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{48C8DF8B-6279-4847-B5FA-E3FCAC2F369F}">
+  <threadedComment ref="B109" dT="2022-12-09T23:25:43.36" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{48C8DF8B-6279-4847-B5FA-E3FCAC2F369F}">
     <text>All other instances of Date_Seeded are 11/21 for SCC</text>
-  </threadedComment>
-  <threadedComment ref="E147" dT="2022-12-09T23:23:32.25" personId="{33287971-19C1-4AC0-9A38-D99609F848BD}" id="{20D10316-DDDD-4B4D-BC95-1D24F680103B}">
-    <text>"Seed" is standardized and used throughout the data otherwise (although technically this does mean the plot only received seeding and no ground modification)</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,13 +1402,13 @@
         <v>44473</v>
       </c>
       <c r="D13">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1434,13 +1422,13 @@
         <v>44473</v>
       </c>
       <c r="D14">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1454,13 +1442,13 @@
         <v>44473</v>
       </c>
       <c r="D15">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1474,30 +1462,30 @@
         <v>44473</v>
       </c>
       <c r="D16">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1">
-        <v>43818</v>
+        <v>11</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43794</v>
       </c>
       <c r="C17" s="1">
-        <v>44473</v>
+        <v>43916</v>
       </c>
       <c r="D17">
-        <v>32</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
@@ -1514,10 +1502,10 @@
         <v>43916</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
@@ -1534,10 +1522,10 @@
         <v>43916</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -1554,10 +1542,10 @@
         <v>43916</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
@@ -1574,13 +1562,13 @@
         <v>43916</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1594,13 +1582,13 @@
         <v>43916</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1614,10 +1602,10 @@
         <v>43916</v>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
@@ -1634,13 +1622,13 @@
         <v>43916</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1654,13 +1642,13 @@
         <v>43916</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1674,13 +1662,13 @@
         <v>43916</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1694,13 +1682,13 @@
         <v>43916</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1714,10 +1702,10 @@
         <v>43916</v>
       </c>
       <c r="D28">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
         <v>9</v>
@@ -1734,13 +1722,13 @@
         <v>43916</v>
       </c>
       <c r="D29">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
         <v>12</v>
       </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
       <c r="F29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1754,10 +1742,10 @@
         <v>43916</v>
       </c>
       <c r="D30">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
@@ -1774,10 +1762,10 @@
         <v>43916</v>
       </c>
       <c r="D31">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -1794,10 +1782,10 @@
         <v>43916</v>
       </c>
       <c r="D32">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -1814,13 +1802,13 @@
         <v>43916</v>
       </c>
       <c r="D33">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1834,10 +1822,10 @@
         <v>43916</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F34" t="s">
         <v>9</v>
@@ -1854,10 +1842,10 @@
         <v>43916</v>
       </c>
       <c r="D35">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
         <v>9</v>
@@ -1874,13 +1862,13 @@
         <v>43916</v>
       </c>
       <c r="D36">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1894,13 +1882,13 @@
         <v>43916</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1914,13 +1902,13 @@
         <v>43916</v>
       </c>
       <c r="D38">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1934,10 +1922,10 @@
         <v>43916</v>
       </c>
       <c r="D39">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
@@ -1954,13 +1942,13 @@
         <v>43916</v>
       </c>
       <c r="D40">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1974,13 +1962,13 @@
         <v>43916</v>
       </c>
       <c r="D41">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1994,10 +1982,10 @@
         <v>43916</v>
       </c>
       <c r="D42">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F42" t="s">
         <v>10</v>
@@ -2014,13 +2002,13 @@
         <v>43916</v>
       </c>
       <c r="D43">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2034,10 +2022,10 @@
         <v>43916</v>
       </c>
       <c r="D44">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
@@ -2054,13 +2042,13 @@
         <v>43916</v>
       </c>
       <c r="D45">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2074,13 +2062,13 @@
         <v>43916</v>
       </c>
       <c r="D46">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2094,10 +2082,10 @@
         <v>43916</v>
       </c>
       <c r="D47">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F47" t="s">
         <v>10</v>
@@ -2114,13 +2102,13 @@
         <v>43916</v>
       </c>
       <c r="D48">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2134,10 +2122,10 @@
         <v>43916</v>
       </c>
       <c r="D49">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
         <v>9</v>
@@ -2154,10 +2142,10 @@
         <v>43916</v>
       </c>
       <c r="D50">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F50" t="s">
         <v>9</v>
@@ -2174,13 +2162,13 @@
         <v>43916</v>
       </c>
       <c r="D51">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F51" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2194,33 +2182,33 @@
         <v>43916</v>
       </c>
       <c r="D52">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E52" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F52" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>43794</v>
       </c>
       <c r="C53" s="1">
-        <v>43916</v>
+        <v>44285</v>
       </c>
       <c r="D53">
-        <v>36</v>
-      </c>
-      <c r="E53" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="F53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2234,13 +2222,13 @@
         <v>44285</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2254,13 +2242,13 @@
         <v>44285</v>
       </c>
       <c r="D55">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2274,13 +2262,13 @@
         <v>44285</v>
       </c>
       <c r="D56">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2294,13 +2282,13 @@
         <v>44285</v>
       </c>
       <c r="D57">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2314,13 +2302,13 @@
         <v>44285</v>
       </c>
       <c r="D58">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2334,13 +2322,13 @@
         <v>44285</v>
       </c>
       <c r="D59">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2354,13 +2342,13 @@
         <v>44285</v>
       </c>
       <c r="D60">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2371,10 +2359,10 @@
         <v>43794</v>
       </c>
       <c r="C61" s="1">
-        <v>44285</v>
+        <v>44475</v>
       </c>
       <c r="D61">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>13</v>
@@ -2385,22 +2373,22 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>11</v>
-      </c>
-      <c r="B62" s="1">
-        <v>43794</v>
+        <v>17</v>
+      </c>
+      <c r="B62" s="2">
+        <v>43791</v>
       </c>
       <c r="C62" s="1">
-        <v>44475</v>
+        <v>43915</v>
       </c>
       <c r="D62">
-        <v>11</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>7</v>
       </c>
       <c r="F62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,10 +2402,10 @@
         <v>43915</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F63" t="s">
         <v>10</v>
@@ -2434,10 +2422,10 @@
         <v>43915</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F64" t="s">
         <v>10</v>
@@ -2454,10 +2442,10 @@
         <v>43915</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F65" t="s">
         <v>10</v>
@@ -2474,13 +2462,13 @@
         <v>43915</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2494,10 +2482,10 @@
         <v>43915</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F67" t="s">
         <v>9</v>
@@ -2514,10 +2502,10 @@
         <v>43915</v>
       </c>
       <c r="D68">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F68" t="s">
         <v>9</v>
@@ -2534,13 +2522,13 @@
         <v>43915</v>
       </c>
       <c r="D69">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
         <v>7</v>
       </c>
-      <c r="E69" t="s">
-        <v>13</v>
-      </c>
       <c r="F69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2554,13 +2542,13 @@
         <v>43915</v>
       </c>
       <c r="D70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2574,13 +2562,13 @@
         <v>43915</v>
       </c>
       <c r="D71">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2594,13 +2582,13 @@
         <v>43915</v>
       </c>
       <c r="D72">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2614,13 +2602,13 @@
         <v>43915</v>
       </c>
       <c r="D73">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2634,13 +2622,13 @@
         <v>43915</v>
       </c>
       <c r="D74">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F74" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2654,10 +2642,10 @@
         <v>43915</v>
       </c>
       <c r="D75">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E75" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F75" t="s">
         <v>9</v>
@@ -2674,13 +2662,13 @@
         <v>43915</v>
       </c>
       <c r="D76">
+        <v>15</v>
+      </c>
+      <c r="E76" t="s">
         <v>14</v>
       </c>
-      <c r="E76" t="s">
-        <v>12</v>
-      </c>
       <c r="F76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2694,13 +2682,13 @@
         <v>43915</v>
       </c>
       <c r="D77">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E77" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2714,13 +2702,13 @@
         <v>43915</v>
       </c>
       <c r="D78">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F78" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2734,10 +2722,10 @@
         <v>43915</v>
       </c>
       <c r="D79">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E79" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F79" t="s">
         <v>10</v>
@@ -2754,10 +2742,10 @@
         <v>43915</v>
       </c>
       <c r="D80">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E80" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F80" t="s">
         <v>10</v>
@@ -2774,10 +2762,10 @@
         <v>43915</v>
       </c>
       <c r="D81">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F81" t="s">
         <v>10</v>
@@ -2794,13 +2782,13 @@
         <v>43915</v>
       </c>
       <c r="D82">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E82" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2814,10 +2802,10 @@
         <v>43915</v>
       </c>
       <c r="D83">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E83" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F83" t="s">
         <v>9</v>
@@ -2834,13 +2822,13 @@
         <v>43915</v>
       </c>
       <c r="D84">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E84" t="s">
         <v>12</v>
       </c>
       <c r="F84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2854,13 +2842,13 @@
         <v>43915</v>
       </c>
       <c r="D85">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E85" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2874,13 +2862,13 @@
         <v>43915</v>
       </c>
       <c r="D86">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E86" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F86" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2894,13 +2882,13 @@
         <v>43915</v>
       </c>
       <c r="D87">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E87" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2914,13 +2902,13 @@
         <v>43915</v>
       </c>
       <c r="D88">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E88" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2934,10 +2922,10 @@
         <v>43915</v>
       </c>
       <c r="D89">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E89" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -2954,10 +2942,10 @@
         <v>43915</v>
       </c>
       <c r="D90">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E90" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F90" t="s">
         <v>10</v>
@@ -2974,13 +2962,13 @@
         <v>43915</v>
       </c>
       <c r="D91">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E91" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2994,10 +2982,10 @@
         <v>43915</v>
       </c>
       <c r="D92">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F92" t="s">
         <v>9</v>
@@ -3014,10 +3002,10 @@
         <v>43915</v>
       </c>
       <c r="D93">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E93" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F93" t="s">
         <v>9</v>
@@ -3034,10 +3022,10 @@
         <v>43915</v>
       </c>
       <c r="D94">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E94" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F94" t="s">
         <v>9</v>
@@ -3054,13 +3042,13 @@
         <v>43915</v>
       </c>
       <c r="D95">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E95" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -3074,13 +3062,13 @@
         <v>43915</v>
       </c>
       <c r="D96">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E96" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F96" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -3094,33 +3082,33 @@
         <v>43915</v>
       </c>
       <c r="D97">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E97" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F97" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>17</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="1">
         <v>43791</v>
       </c>
       <c r="C98" s="1">
-        <v>43915</v>
+        <v>44287</v>
       </c>
       <c r="D98">
-        <v>36</v>
-      </c>
-      <c r="E98" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F98" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -3134,13 +3122,13 @@
         <v>44287</v>
       </c>
       <c r="D99">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3154,13 +3142,13 @@
         <v>44287</v>
       </c>
       <c r="D100">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F100" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3174,13 +3162,13 @@
         <v>44287</v>
       </c>
       <c r="D101">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -3194,13 +3182,13 @@
         <v>44287</v>
       </c>
       <c r="D102">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F102" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -3214,13 +3202,13 @@
         <v>44287</v>
       </c>
       <c r="D103">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -3234,13 +3222,13 @@
         <v>44287</v>
       </c>
       <c r="D104">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F104" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,13 +3242,13 @@
         <v>44287</v>
       </c>
       <c r="D105">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -3271,16 +3259,16 @@
         <v>43791</v>
       </c>
       <c r="C106" s="1">
-        <v>44287</v>
+        <v>44477</v>
       </c>
       <c r="D106">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F106" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -3294,13 +3282,13 @@
         <v>44477</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -3314,7 +3302,7 @@
         <v>44477</v>
       </c>
       <c r="D108">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>13</v>
@@ -3325,39 +3313,39 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>17</v>
-      </c>
-      <c r="B109" s="1">
-        <v>43791</v>
+        <v>18</v>
+      </c>
+      <c r="B109" s="2">
+        <v>43790</v>
       </c>
       <c r="C109" s="1">
-        <v>44477</v>
+        <v>43917</v>
       </c>
       <c r="D109">
-        <v>30</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>12</v>
       </c>
       <c r="F109" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>17</v>
-      </c>
-      <c r="B110" s="1">
-        <v>43791</v>
+        <v>18</v>
+      </c>
+      <c r="B110" s="2">
+        <v>43790</v>
       </c>
       <c r="C110" s="1">
-        <v>44477</v>
+        <v>43917</v>
       </c>
       <c r="D110">
-        <v>34</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>14</v>
       </c>
       <c r="F110" t="s">
         <v>10</v>
@@ -3374,13 +3362,13 @@
         <v>43917</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E111" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F111" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -3394,10 +3382,10 @@
         <v>43917</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F112" t="s">
         <v>10</v>
@@ -3414,13 +3402,13 @@
         <v>43917</v>
       </c>
       <c r="D113">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E113" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F113" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3434,13 +3422,13 @@
         <v>43917</v>
       </c>
       <c r="D114">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3454,13 +3442,13 @@
         <v>43917</v>
       </c>
       <c r="D115">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E115" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3474,10 +3462,10 @@
         <v>43917</v>
       </c>
       <c r="D116">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E116" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F116" t="s">
         <v>9</v>
@@ -3494,13 +3482,13 @@
         <v>43917</v>
       </c>
       <c r="D117">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E117" t="s">
         <v>12</v>
       </c>
       <c r="F117" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3514,10 +3502,10 @@
         <v>43917</v>
       </c>
       <c r="D118">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E118" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F118" t="s">
         <v>9</v>
@@ -3534,10 +3522,10 @@
         <v>43917</v>
       </c>
       <c r="D119">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E119" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F119" t="s">
         <v>10</v>
@@ -3554,13 +3542,13 @@
         <v>43917</v>
       </c>
       <c r="D120">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E120" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F120" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3574,10 +3562,10 @@
         <v>43917</v>
       </c>
       <c r="D121">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F121" t="s">
         <v>10</v>
@@ -3594,13 +3582,13 @@
         <v>43917</v>
       </c>
       <c r="D122">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E122" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F122" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3614,13 +3602,13 @@
         <v>43917</v>
       </c>
       <c r="D123">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E123" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F123" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3634,10 +3622,10 @@
         <v>43917</v>
       </c>
       <c r="D124">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E124" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F124" t="s">
         <v>9</v>
@@ -3654,13 +3642,13 @@
         <v>43917</v>
       </c>
       <c r="D125">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E125" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F125" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3674,13 +3662,13 @@
         <v>43917</v>
       </c>
       <c r="D126">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E126" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F126" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3694,13 +3682,13 @@
         <v>43917</v>
       </c>
       <c r="D127">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E127" t="s">
         <v>12</v>
       </c>
       <c r="F127" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3714,10 +3702,10 @@
         <v>43917</v>
       </c>
       <c r="D128">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E128" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F128" t="s">
         <v>10</v>
@@ -3734,13 +3722,13 @@
         <v>43917</v>
       </c>
       <c r="D129">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E129" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F129" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3754,10 +3742,10 @@
         <v>43917</v>
       </c>
       <c r="D130">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E130" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F130" t="s">
         <v>10</v>
@@ -3774,10 +3762,10 @@
         <v>43917</v>
       </c>
       <c r="D131">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E131" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F131" t="s">
         <v>9</v>
@@ -3794,10 +3782,10 @@
         <v>43917</v>
       </c>
       <c r="D132">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E132" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F132" t="s">
         <v>10</v>
@@ -3814,10 +3802,10 @@
         <v>43917</v>
       </c>
       <c r="D133">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F133" t="s">
         <v>9</v>
@@ -3834,10 +3822,10 @@
         <v>43917</v>
       </c>
       <c r="D134">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E134" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -3854,10 +3842,10 @@
         <v>43917</v>
       </c>
       <c r="D135">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E135" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F135" t="s">
         <v>9</v>
@@ -3874,13 +3862,13 @@
         <v>43917</v>
       </c>
       <c r="D136">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E136" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F136" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3894,13 +3882,13 @@
         <v>43917</v>
       </c>
       <c r="D137">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E137" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F137" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3914,13 +3902,13 @@
         <v>43917</v>
       </c>
       <c r="D138">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E138" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F138" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3934,13 +3922,13 @@
         <v>43917</v>
       </c>
       <c r="D139">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E139" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F139" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -3954,10 +3942,10 @@
         <v>43917</v>
       </c>
       <c r="D140">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E140" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F140" t="s">
         <v>10</v>
@@ -3974,13 +3962,13 @@
         <v>43917</v>
       </c>
       <c r="D141">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E141" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F141" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -3994,13 +3982,13 @@
         <v>43917</v>
       </c>
       <c r="D142">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E142" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F142" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -4014,10 +4002,10 @@
         <v>43917</v>
       </c>
       <c r="D143">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E143" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F143" t="s">
         <v>9</v>
@@ -4034,10 +4022,10 @@
         <v>43917</v>
       </c>
       <c r="D144">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E144" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F144" t="s">
         <v>9</v>
@@ -4047,37 +4035,37 @@
       <c r="A145" t="s">
         <v>18</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B145" s="1">
         <v>43790</v>
       </c>
       <c r="C145" s="1">
-        <v>43917</v>
+        <v>44286</v>
       </c>
       <c r="D145">
-        <v>35</v>
-      </c>
-      <c r="E145" t="s">
+        <v>32</v>
+      </c>
+      <c r="E145" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F145" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>18</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B146" s="1">
         <v>43790</v>
       </c>
       <c r="C146" s="1">
-        <v>43917</v>
+        <v>44482</v>
       </c>
       <c r="D146">
-        <v>36</v>
-      </c>
-      <c r="E146" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="F146" t="s">
         <v>9</v>
@@ -4087,20 +4075,20 @@
       <c r="A147" t="s">
         <v>18</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B147" s="1">
         <v>43790</v>
       </c>
       <c r="C147" s="1">
-        <v>44286</v>
+        <v>44482</v>
       </c>
       <c r="D147">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F147" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -4111,195 +4099,15 @@
         <v>43790</v>
       </c>
       <c r="C148" s="1">
-        <v>44286</v>
+        <v>44482</v>
       </c>
       <c r="D148">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F148" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>18</v>
-      </c>
-      <c r="B149" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C149" s="1">
-        <v>44286</v>
-      </c>
-      <c r="D149">
-        <v>13</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F149" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>18</v>
-      </c>
-      <c r="B150" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C150" s="1">
-        <v>44286</v>
-      </c>
-      <c r="D150">
-        <v>16</v>
-      </c>
-      <c r="E150" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F150" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>18</v>
-      </c>
-      <c r="B151" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C151" s="1">
-        <v>44286</v>
-      </c>
-      <c r="D151">
-        <v>22</v>
-      </c>
-      <c r="E151" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F151" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>18</v>
-      </c>
-      <c r="B152" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C152" s="1">
-        <v>44286</v>
-      </c>
-      <c r="D152">
-        <v>25</v>
-      </c>
-      <c r="E152" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F152" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>18</v>
-      </c>
-      <c r="B153" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C153" s="1">
-        <v>44286</v>
-      </c>
-      <c r="D153">
-        <v>32</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F153" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>18</v>
-      </c>
-      <c r="B154" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C154" s="1">
-        <v>44286</v>
-      </c>
-      <c r="D154">
-        <v>35</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F154" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>18</v>
-      </c>
-      <c r="B155" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C155" s="1">
-        <v>44482</v>
-      </c>
-      <c r="D155">
-        <v>16</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F155" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>18</v>
-      </c>
-      <c r="B156" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C156" s="1">
-        <v>44482</v>
-      </c>
-      <c r="D156">
-        <v>25</v>
-      </c>
-      <c r="E156" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F156" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
-        <v>18</v>
-      </c>
-      <c r="B157" s="1">
-        <v>43790</v>
-      </c>
-      <c r="C157" s="1">
-        <v>44482</v>
-      </c>
-      <c r="D157">
-        <v>35</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F157" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>